<commit_message>
forgot to adjust values for day 1
</commit_message>
<xml_diff>
--- a/D3/Sprint #1 - Sprint Backlog.xlsx
+++ b/D3/Sprint #1 - Sprint Backlog.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="32">
   <si>
     <t>As Natalie, a Historian, I want a checklist prompt to save changes across all identical files in all directories so my files are consistent</t>
   </si>
@@ -139,7 +139,22 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>3.5</t>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">v: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
     </r>
   </si>
 </sst>
@@ -401,27 +416,27 @@
   <autoFilter ref="B17:P24"/>
   <tableColumns count="15">
     <tableColumn id="1" name="Tasks" dataDxfId="15"/>
-    <tableColumn id="2" name="Day 1" dataDxfId="13"/>
-    <tableColumn id="3" name="Day 2" dataDxfId="12"/>
-    <tableColumn id="4" name="Day 3" dataDxfId="11"/>
-    <tableColumn id="5" name="Day 4" dataDxfId="10"/>
-    <tableColumn id="6" name="Day 5" dataDxfId="9"/>
-    <tableColumn id="7" name="Day 6" dataDxfId="8"/>
-    <tableColumn id="8" name="Day 7" dataDxfId="7"/>
-    <tableColumn id="9" name="Day 8" dataDxfId="6"/>
-    <tableColumn id="10" name="Day 9" dataDxfId="5"/>
-    <tableColumn id="11" name="Day 10" dataDxfId="4"/>
-    <tableColumn id="12" name="Day 11" dataDxfId="3"/>
-    <tableColumn id="13" name="Day 12" dataDxfId="2"/>
-    <tableColumn id="14" name="Day 13" dataDxfId="1"/>
-    <tableColumn id="15" name="Day 14" dataDxfId="0"/>
+    <tableColumn id="2" name="Day 1" dataDxfId="14"/>
+    <tableColumn id="3" name="Day 2" dataDxfId="13"/>
+    <tableColumn id="4" name="Day 3" dataDxfId="12"/>
+    <tableColumn id="5" name="Day 4" dataDxfId="11"/>
+    <tableColumn id="6" name="Day 5" dataDxfId="10"/>
+    <tableColumn id="7" name="Day 6" dataDxfId="9"/>
+    <tableColumn id="8" name="Day 7" dataDxfId="8"/>
+    <tableColumn id="9" name="Day 8" dataDxfId="7"/>
+    <tableColumn id="10" name="Day 9" dataDxfId="6"/>
+    <tableColumn id="11" name="Day 10" dataDxfId="5"/>
+    <tableColumn id="12" name="Day 11" dataDxfId="4"/>
+    <tableColumn id="13" name="Day 12" dataDxfId="3"/>
+    <tableColumn id="14" name="Day 13" dataDxfId="2"/>
+    <tableColumn id="15" name="Day 14" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table83" displayName="Table83" ref="S17:S24" totalsRowShown="0" headerRowDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table83" displayName="Table83" ref="S17:S24" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="S17:S24"/>
   <tableColumns count="1">
     <tableColumn id="1" name="Task Sum">
@@ -698,7 +713,7 @@
   <dimension ref="A1:S29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1272,7 +1287,7 @@
         <v>18</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D18" s="1">
         <v>3.5</v>

</xml_diff>

<commit_message>
Revert "Updated Sprint Backlog"
This reverts commit 1dc9a1207b02051a95062870ad9628c0d3cc74ed.
</commit_message>
<xml_diff>
--- a/D3/Sprint #1 - Sprint Backlog.xlsx
+++ b/D3/Sprint #1 - Sprint Backlog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nanson\Desktop\Homework\University\CSCC01\team14-course-project\D3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows\Documents\GitHub\team14-course-project\D3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="38">
   <si>
     <t>Estimated</t>
   </si>
@@ -339,28 +339,13 @@
       </rPr>
       <t>1</t>
     </r>
-  </si>
-  <si>
-    <r>
-      <t>N:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <phoneticPr fontId="6"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -906,22 +891,22 @@
   <dimension ref="A1:S29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.7109375" customWidth="1"/>
     <col min="2" max="2" width="44.28515625" customWidth="1"/>
     <col min="19" max="19" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="14.45" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -974,7 +959,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19">
       <c r="A3" s="10" t="s">
         <v>18</v>
       </c>
@@ -1028,7 +1013,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19">
       <c r="A4" s="10"/>
       <c r="B4" s="2" t="s">
         <v>20</v>
@@ -1080,7 +1065,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19">
       <c r="A5" s="10"/>
       <c r="B5" s="2" t="s">
         <v>21</v>
@@ -1132,7 +1117,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19">
       <c r="A6" s="10"/>
       <c r="B6" s="2" t="s">
         <v>22</v>
@@ -1184,7 +1169,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19">
       <c r="A7" s="10"/>
       <c r="B7" s="2" t="s">
         <v>23</v>
@@ -1236,7 +1221,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19">
       <c r="A8" s="10"/>
       <c r="B8" s="2" t="s">
         <v>24</v>
@@ -1288,7 +1273,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19">
       <c r="A9" s="10"/>
       <c r="B9" s="2" t="s">
         <v>25</v>
@@ -1340,7 +1325,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19">
       <c r="A12" s="3" t="s">
         <v>26</v>
       </c>
@@ -1402,7 +1387,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19">
       <c r="A14" s="5" t="s">
         <v>27</v>
       </c>
@@ -1411,7 +1396,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -1419,7 +1404,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19">
       <c r="A17" s="1" t="s">
         <v>1</v>
       </c>
@@ -1472,7 +1457,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19">
       <c r="A18" s="10" t="s">
         <v>18</v>
       </c>
@@ -1509,7 +1494,7 @@
       <c r="L18" s="2">
         <v>1.5</v>
       </c>
-      <c r="M18" s="8">
+      <c r="M18" s="2">
         <v>1.5</v>
       </c>
       <c r="N18" s="2">
@@ -1526,7 +1511,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19">
       <c r="A19" s="10"/>
       <c r="B19" s="2" t="s">
         <v>20</v>
@@ -1561,8 +1546,8 @@
       <c r="L19" s="2">
         <v>1</v>
       </c>
-      <c r="M19" s="8" t="s">
-        <v>38</v>
+      <c r="M19" s="2">
+        <v>1</v>
       </c>
       <c r="N19" s="2">
         <v>2</v>
@@ -1575,10 +1560,10 @@
       </c>
       <c r="S19">
         <f t="shared" ref="S19" si="3">SUM(C19:P19)</f>
-        <v>12.5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19">
       <c r="A20" s="10"/>
       <c r="B20" s="2" t="s">
         <v>21</v>
@@ -1630,7 +1615,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19">
       <c r="A21" s="10"/>
       <c r="B21" s="2" t="s">
         <v>22</v>
@@ -1682,7 +1667,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19">
       <c r="A22" s="10"/>
       <c r="B22" s="2" t="s">
         <v>23</v>
@@ -1734,7 +1719,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19">
       <c r="A23" s="10"/>
       <c r="B23" s="2" t="s">
         <v>24</v>
@@ -1786,7 +1771,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19">
       <c r="A24" s="10"/>
       <c r="B24" s="2" t="s">
         <v>25</v>
@@ -1838,7 +1823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19">
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
@@ -1885,7 +1870,7 @@
       </c>
       <c r="M27" s="4">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N27" s="4">
         <f t="shared" si="5"/>
@@ -1900,13 +1885,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19">
       <c r="A29" s="5" t="s">
         <v>27</v>
       </c>
       <c r="B29" s="6">
         <f>SUM(C27:P27)</f>
-        <v>68.5</v>
+        <v>69.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Retry - Updated Sprint Backlog
I'm thinking of building the plugin from scratch than modifying the
hello world code.
</commit_message>
<xml_diff>
--- a/D3/Sprint #1 - Sprint Backlog.xlsx
+++ b/D3/Sprint #1 - Sprint Backlog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows\Documents\GitHub\team14-course-project\D3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nanson\Desktop\Homework\University\CSCC01\team14-course-project\D3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="39">
   <si>
     <t>Estimated</t>
   </si>
@@ -339,13 +339,37 @@
       </rPr>
       <t>1</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t>N</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 2</t>
+    </r>
+    <phoneticPr fontId="6"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -891,22 +915,22 @@
   <dimension ref="A1:S29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.7109375" customWidth="1"/>
     <col min="2" max="2" width="44.28515625" customWidth="1"/>
     <col min="19" max="19" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="14.45" customHeight="1">
+    <row r="2" spans="1:19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -959,7 +983,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>18</v>
       </c>
@@ -1013,7 +1037,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
       <c r="B4" s="2" t="s">
         <v>20</v>
@@ -1065,7 +1089,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" s="2" t="s">
         <v>21</v>
@@ -1117,7 +1141,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="10"/>
       <c r="B6" s="2" t="s">
         <v>22</v>
@@ -1169,7 +1193,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
       <c r="B7" s="2" t="s">
         <v>23</v>
@@ -1221,7 +1245,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
       <c r="B8" s="2" t="s">
         <v>24</v>
@@ -1273,7 +1297,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
       <c r="B9" s="2" t="s">
         <v>25</v>
@@ -1325,7 +1349,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>26</v>
       </c>
@@ -1387,7 +1411,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>27</v>
       </c>
@@ -1396,7 +1420,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -1404,7 +1428,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:19">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>1</v>
       </c>
@@ -1457,7 +1481,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:19">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>18</v>
       </c>
@@ -1511,7 +1535,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:19">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
       <c r="B19" s="2" t="s">
         <v>20</v>
@@ -1543,8 +1567,8 @@
       <c r="K19" s="2">
         <v>1</v>
       </c>
-      <c r="L19" s="2">
-        <v>1</v>
+      <c r="L19" s="8" t="s">
+        <v>38</v>
       </c>
       <c r="M19" s="2">
         <v>1</v>
@@ -1560,10 +1584,10 @@
       </c>
       <c r="S19">
         <f t="shared" ref="S19" si="3">SUM(C19:P19)</f>
-        <v>13.5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
       <c r="B20" s="2" t="s">
         <v>21</v>
@@ -1615,7 +1639,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:19">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
       <c r="B21" s="2" t="s">
         <v>22</v>
@@ -1667,7 +1691,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:19">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
       <c r="B22" s="2" t="s">
         <v>23</v>
@@ -1719,7 +1743,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:19">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="10"/>
       <c r="B23" s="2" t="s">
         <v>24</v>
@@ -1771,7 +1795,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:19">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="10"/>
       <c r="B24" s="2" t="s">
         <v>25</v>
@@ -1823,7 +1847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:19">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
@@ -1866,7 +1890,7 @@
       </c>
       <c r="L27" s="4">
         <f t="shared" si="5"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M27" s="4">
         <f t="shared" si="5"/>
@@ -1885,13 +1909,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:19">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>27</v>
       </c>
       <c r="B29" s="6">
         <f>SUM(C27:P27)</f>
-        <v>69.5</v>
+        <v>68.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Install working on Zotero Standalone, but no functionality yet
</commit_message>
<xml_diff>
--- a/D3/Sprint #1 - Sprint Backlog.xlsx
+++ b/D3/Sprint #1 - Sprint Backlog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nanson\Desktop\Homework\University\CSCC01\team14-course-project\D3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows\Documents\GitHub\team14-course-project\D3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="39">
   <si>
     <t>Estimated</t>
   </si>
@@ -369,7 +369,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -915,22 +915,22 @@
   <dimension ref="A1:S29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.7109375" customWidth="1"/>
     <col min="2" max="2" width="44.28515625" customWidth="1"/>
     <col min="19" max="19" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="14.45" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -983,7 +983,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19">
       <c r="A3" s="10" t="s">
         <v>18</v>
       </c>
@@ -1037,7 +1037,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19">
       <c r="A4" s="10"/>
       <c r="B4" s="2" t="s">
         <v>20</v>
@@ -1089,7 +1089,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19">
       <c r="A5" s="10"/>
       <c r="B5" s="2" t="s">
         <v>21</v>
@@ -1141,7 +1141,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19">
       <c r="A6" s="10"/>
       <c r="B6" s="2" t="s">
         <v>22</v>
@@ -1193,7 +1193,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19">
       <c r="A7" s="10"/>
       <c r="B7" s="2" t="s">
         <v>23</v>
@@ -1245,7 +1245,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19">
       <c r="A8" s="10"/>
       <c r="B8" s="2" t="s">
         <v>24</v>
@@ -1297,7 +1297,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19">
       <c r="A9" s="10"/>
       <c r="B9" s="2" t="s">
         <v>25</v>
@@ -1349,7 +1349,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19">
       <c r="A12" s="3" t="s">
         <v>26</v>
       </c>
@@ -1411,7 +1411,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19">
       <c r="A14" s="5" t="s">
         <v>27</v>
       </c>
@@ -1420,7 +1420,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -1428,7 +1428,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19">
       <c r="A17" s="1" t="s">
         <v>1</v>
       </c>
@@ -1481,7 +1481,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19">
       <c r="A18" s="10" t="s">
         <v>18</v>
       </c>
@@ -1515,8 +1515,8 @@
       <c r="K18" s="2">
         <v>1</v>
       </c>
-      <c r="L18" s="2">
-        <v>1.5</v>
+      <c r="L18" s="8" t="s">
+        <v>37</v>
       </c>
       <c r="M18" s="2">
         <v>1.5</v>
@@ -1532,10 +1532,10 @@
       </c>
       <c r="S18">
         <f>SUM(C18:P18)</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19">
       <c r="A19" s="10"/>
       <c r="B19" s="2" t="s">
         <v>20</v>
@@ -1587,7 +1587,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19">
       <c r="A20" s="10"/>
       <c r="B20" s="2" t="s">
         <v>21</v>
@@ -1639,7 +1639,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19">
       <c r="A21" s="10"/>
       <c r="B21" s="2" t="s">
         <v>22</v>
@@ -1691,7 +1691,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19">
       <c r="A22" s="10"/>
       <c r="B22" s="2" t="s">
         <v>23</v>
@@ -1743,7 +1743,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19">
       <c r="A23" s="10"/>
       <c r="B23" s="2" t="s">
         <v>24</v>
@@ -1795,7 +1795,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19">
       <c r="A24" s="10"/>
       <c r="B24" s="2" t="s">
         <v>25</v>
@@ -1847,7 +1847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19">
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
@@ -1890,7 +1890,7 @@
       </c>
       <c r="L27" s="4">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>4.5</v>
       </c>
       <c r="M27" s="4">
         <f t="shared" si="5"/>
@@ -1909,13 +1909,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19">
       <c r="A29" s="5" t="s">
         <v>27</v>
       </c>
       <c r="B29" s="6">
         <f>SUM(C27:P27)</f>
-        <v>68.5</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created sprint documentation file
</commit_message>
<xml_diff>
--- a/D3/Sprint #1 - Sprint Backlog.xlsx
+++ b/D3/Sprint #1 - Sprint Backlog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="39">
   <si>
     <t>Estimated</t>
   </si>
@@ -240,13 +240,69 @@
   </si>
   <si>
     <r>
+      <t>N</t>
+    </r>
+    <r>
       <rPr>
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">Vincent Ho </t>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">V: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>N</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 2</t>
+    </r>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Vincent Ho: </t>
     </r>
     <r>
       <rPr>
@@ -263,7 +319,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>Robbie Rao</t>
+      <t>Robbie Rao:</t>
     </r>
     <r>
       <rPr>
@@ -289,7 +345,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">Nanson Zheng </t>
+      <t xml:space="preserve">Nanson Zheng: </t>
     </r>
     <r>
       <rPr>
@@ -300,69 +356,6 @@
       </rPr>
       <t>Green</t>
     </r>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <r>
-      <t>N</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>3</t>
-    </r>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">V: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>N</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> 2</t>
-    </r>
-    <phoneticPr fontId="6"/>
   </si>
 </sst>
 </file>
@@ -516,7 +509,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table5" displayName="Table5" ref="B2:P9" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table510" displayName="Table510" ref="B2:P9" headerRowCount="0">
   <tableColumns count="15">
     <tableColumn id="1" name="Column1"/>
     <tableColumn id="2" name="Column2"/>
@@ -539,7 +532,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table8" displayName="Table8" ref="S2:S9" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table811" displayName="Table811" ref="S2:S9" headerRowCount="0">
   <tableColumns count="1">
     <tableColumn id="1" name="Column1">
       <calculatedColumnFormula>SUM(C2:P2)</calculatedColumnFormula>
@@ -550,7 +543,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table52" displayName="Table52" ref="B17:P24" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table5212" displayName="Table5212" ref="B17:P24" headerRowCount="0">
   <tableColumns count="15">
     <tableColumn id="1" name="Column1"/>
     <tableColumn id="2" name="Column2"/>
@@ -573,7 +566,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table83" displayName="Table83" ref="S17:S24" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table8313" displayName="Table8313" ref="S17:S24" headerRowCount="0">
   <tableColumns count="1">
     <tableColumn id="1" name="Column1">
       <calculatedColumnFormula>SUM(C17:P17)</calculatedColumnFormula>
@@ -912,21 +905,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S29"/>
+  <dimension ref="A1:S27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.7109375" customWidth="1"/>
     <col min="2" max="2" width="44.28515625" customWidth="1"/>
+    <col min="3" max="3" width="9" customWidth="1"/>
     <col min="19" max="19" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
-      <c r="A1" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
     </row>
@@ -983,7 +977,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" s="10" t="s">
         <v>18</v>
       </c>
@@ -1037,7 +1031,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" ht="15" customHeight="1">
       <c r="A4" s="10"/>
       <c r="B4" s="2" t="s">
         <v>20</v>
@@ -1355,59 +1349,59 @@
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4">
-        <f t="shared" ref="C12" si="1">SUM(C3:C9)</f>
+        <f t="shared" ref="C12:P12" si="1">SUM(C3:C9)</f>
         <v>7</v>
       </c>
       <c r="D12" s="4">
-        <f t="shared" ref="D12:P12" si="2">SUM(D3:D9)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="E12" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="F12" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="G12" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="H12" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="I12" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="J12" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="K12" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="L12" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="M12" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="N12" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="O12" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="P12" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
     </row>
@@ -1425,7 +1419,7 @@
         <v>28</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:19">
@@ -1481,7 +1475,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:19">
+    <row r="18" spans="1:19" ht="15" customHeight="1">
       <c r="A18" s="10" t="s">
         <v>18</v>
       </c>
@@ -1504,19 +1498,19 @@
         <v>34</v>
       </c>
       <c r="H18" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M18" s="2">
         <v>1.5</v>
@@ -1532,10 +1526,10 @@
       </c>
       <c r="S18">
         <f>SUM(C18:P18)</f>
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" ht="15" customHeight="1">
       <c r="A19" s="10"/>
       <c r="B19" s="2" t="s">
         <v>20</v>
@@ -1547,28 +1541,28 @@
         <v>33</v>
       </c>
       <c r="E19" s="2">
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>32</v>
       </c>
       <c r="G19" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I19" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J19" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K19" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L19" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M19" s="2">
         <v>1</v>
@@ -1583,8 +1577,8 @@
         <v>1</v>
       </c>
       <c r="S19">
-        <f t="shared" ref="S19" si="3">SUM(C19:P19)</f>
-        <v>12.5</v>
+        <f t="shared" ref="S19" si="2">SUM(C19:P19)</f>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:19">
@@ -1599,25 +1593,25 @@
         <v>0</v>
       </c>
       <c r="E20" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G20" s="2">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="H20" s="2">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="I20" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J20" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K20" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L20" s="2">
         <v>0</v>
@@ -1636,7 +1630,7 @@
       </c>
       <c r="S20">
         <f>SUM(C20:P20)</f>
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:19">
@@ -1669,10 +1663,10 @@
         <v>0</v>
       </c>
       <c r="K21" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L21" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M21" s="2">
         <v>1</v>
@@ -1688,7 +1682,7 @@
       </c>
       <c r="S21">
         <f>SUM(C21:P21)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:19">
@@ -1703,28 +1697,28 @@
         <v>0</v>
       </c>
       <c r="E22" s="2">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F22" s="2">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G22" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H22" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I22" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J22" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K22" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L22" s="2">
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="M22" s="2">
         <v>2.5</v>
@@ -1740,7 +1734,7 @@
       </c>
       <c r="S22">
         <f>SUM(C22:P22)</f>
-        <v>20</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="23" spans="1:19">
@@ -1755,28 +1749,28 @@
         <v>0</v>
       </c>
       <c r="E23" s="2">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F23" s="2">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G23" s="2">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H23" s="2">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="I23" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J23" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K23" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L23" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M23" s="2">
         <v>1</v>
@@ -1792,7 +1786,7 @@
       </c>
       <c r="S23">
         <f>SUM(C23:P23)</f>
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:19">
@@ -1853,69 +1847,60 @@
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="4">
-        <f t="shared" ref="C27" si="4">SUM(C18:C24)</f>
+        <f t="shared" ref="C27:P27" si="3">SUM(C18:C24)</f>
         <v>0</v>
       </c>
       <c r="D27" s="4">
-        <f t="shared" ref="D27:P27" si="5">SUM(D18:D24)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E27" s="4">
-        <f t="shared" si="5"/>
-        <v>4.5</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="F27" s="4">
-        <f t="shared" si="5"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="G27" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H27" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I27" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J27" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K27" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L27" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M27" s="4">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="N27" s="4">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="O27" s="4">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="P27" s="4">
+        <f t="shared" si="3"/>
         <v>5</v>
-      </c>
-      <c r="H27" s="4">
-        <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="I27" s="4">
-        <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
-      <c r="J27" s="4">
-        <f t="shared" si="5"/>
-        <v>7</v>
-      </c>
-      <c r="K27" s="4">
-        <f t="shared" si="5"/>
-        <v>7</v>
-      </c>
-      <c r="L27" s="4">
-        <f t="shared" si="5"/>
-        <v>4.5</v>
-      </c>
-      <c r="M27" s="4">
-        <f t="shared" si="5"/>
-        <v>7</v>
-      </c>
-      <c r="N27" s="4">
-        <f t="shared" si="5"/>
-        <v>7</v>
-      </c>
-      <c r="O27" s="4">
-        <f t="shared" si="5"/>
-        <v>7</v>
-      </c>
-      <c r="P27" s="4">
-        <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19">
-      <c r="A29" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B29" s="6">
-        <f>SUM(C27:P27)</f>
-        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Logged work hours for D3
</commit_message>
<xml_diff>
--- a/D3/Sprint #1 - Sprint Backlog.xlsx
+++ b/D3/Sprint #1 - Sprint Backlog.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kirisanth\School\CSCC01\team14-course-project\D3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mitko\Documents\team14-course-project\D3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22956" windowHeight="9840"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22950" windowHeight="9840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="45">
   <si>
     <t>Estimated</t>
   </si>
@@ -448,6 +448,23 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve"> 1</t>
+    </r>
+  </si>
+  <si>
+    <t>Dimitar Stratiev</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">D: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>2.5</t>
     </r>
   </si>
 </sst>
@@ -455,7 +472,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -506,6 +523,12 @@
     <font>
       <sz val="11"/>
       <color theme="3" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -568,7 +591,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -587,6 +610,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1003,16 +1027,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S24" sqref="S24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" customWidth="1"/>
-    <col min="2" max="2" width="44.33203125" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="44.28515625" customWidth="1"/>
     <col min="3" max="3" width="9" customWidth="1"/>
-    <col min="19" max="19" width="10.44140625" customWidth="1"/>
+    <col min="19" max="19" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -1020,7 +1044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="14.4" customHeight="1">
+    <row r="2" spans="1:19" ht="14.45" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1517,6 +1541,9 @@
       <c r="B16" s="8" t="s">
         <v>36</v>
       </c>
+      <c r="H16" s="10" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="17" spans="1:19">
       <c r="A17" s="1" t="s">
@@ -1621,8 +1648,7 @@
         <v>1</v>
       </c>
       <c r="S18">
-        <f>SUM(C18:P18)</f>
-        <v>4.5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:19" ht="15" customHeight="1">
@@ -1673,8 +1699,7 @@
         <v>41</v>
       </c>
       <c r="S19">
-        <f t="shared" ref="S19" si="2">SUM(C19:P19)</f>
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:19">
@@ -1773,12 +1798,11 @@
       <c r="O21" s="2">
         <v>1</v>
       </c>
-      <c r="P21" s="2">
-        <v>0</v>
+      <c r="P21" s="7" t="s">
+        <v>44</v>
       </c>
       <c r="S21">
-        <f>SUM(C21:P21)</f>
-        <v>3</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="22" spans="1:19">
@@ -1829,8 +1853,7 @@
         <v>39</v>
       </c>
       <c r="S22">
-        <f>SUM(C22:P22)</f>
-        <v>0</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="23" spans="1:19">
@@ -1881,7 +1904,6 @@
         <v>1</v>
       </c>
       <c r="S23">
-        <f>SUM(C23:P23)</f>
         <v>4</v>
       </c>
     </row>
@@ -1943,60 +1965,48 @@
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="4">
-        <f t="shared" ref="C27:P27" si="3">SUM(C18:C24)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D27" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E27" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="F27" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G27" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H27" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I27" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J27" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K27" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L27" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M27" s="4">
-        <f t="shared" si="3"/>
-        <v>4.5</v>
+        <v>7</v>
       </c>
       <c r="N27" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="C27:P27" si="2">SUM(N18:N24)</f>
         <v>3</v>
       </c>
       <c r="O27" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="P27" s="4">
-        <f t="shared" si="3"/>
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
merged Dimitar's GUI plugin with my plugin, updated Spring Documentation
</commit_message>
<xml_diff>
--- a/D3/Sprint #1 - Sprint Backlog.xlsx
+++ b/D3/Sprint #1 - Sprint Backlog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mitko\Documents\team14-course-project\D3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows\Documents\GitHub\team14-course-project\D3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="46">
   <si>
     <t>Estimated</t>
   </si>
@@ -465,6 +465,20 @@
         <family val="2"/>
       </rPr>
       <t>2.5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">V: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
     </r>
   </si>
 </sst>
@@ -607,10 +621,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1028,7 +1042,7 @@
   <dimension ref="A1:S27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S24" sqref="S24"/>
+      <selection activeCell="R23" sqref="R23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1098,7 +1112,7 @@
       </c>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="10" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1152,7 +1166,7 @@
       </c>
     </row>
     <row r="4" spans="1:19" ht="15" customHeight="1">
-      <c r="A4" s="9"/>
+      <c r="A4" s="10"/>
       <c r="B4" s="2" t="s">
         <v>20</v>
       </c>
@@ -1204,7 +1218,7 @@
       </c>
     </row>
     <row r="5" spans="1:19">
-      <c r="A5" s="9"/>
+      <c r="A5" s="10"/>
       <c r="B5" s="2" t="s">
         <v>21</v>
       </c>
@@ -1256,7 +1270,7 @@
       </c>
     </row>
     <row r="6" spans="1:19">
-      <c r="A6" s="9"/>
+      <c r="A6" s="10"/>
       <c r="B6" s="2" t="s">
         <v>22</v>
       </c>
@@ -1308,7 +1322,7 @@
       </c>
     </row>
     <row r="7" spans="1:19">
-      <c r="A7" s="9"/>
+      <c r="A7" s="10"/>
       <c r="B7" s="2" t="s">
         <v>23</v>
       </c>
@@ -1360,7 +1374,7 @@
       </c>
     </row>
     <row r="8" spans="1:19">
-      <c r="A8" s="9"/>
+      <c r="A8" s="10"/>
       <c r="B8" s="2" t="s">
         <v>24</v>
       </c>
@@ -1412,7 +1426,7 @@
       </c>
     </row>
     <row r="9" spans="1:19">
-      <c r="A9" s="9"/>
+      <c r="A9" s="10"/>
       <c r="B9" s="2" t="s">
         <v>25</v>
       </c>
@@ -1541,7 +1555,7 @@
       <c r="B16" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="H16" s="10" t="s">
+      <c r="H16" s="9" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1599,7 +1613,7 @@
       </c>
     </row>
     <row r="18" spans="1:19" ht="15" customHeight="1">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="10" t="s">
         <v>18</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -1636,23 +1650,23 @@
         <v>34</v>
       </c>
       <c r="M18" s="2">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="N18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S18">
         <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:19" ht="15" customHeight="1">
-      <c r="A19" s="9"/>
+      <c r="A19" s="10"/>
       <c r="B19" s="2" t="s">
         <v>20</v>
       </c>
@@ -1687,7 +1701,7 @@
         <v>35</v>
       </c>
       <c r="M19" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N19" s="7">
         <v>0</v>
@@ -1703,7 +1717,7 @@
       </c>
     </row>
     <row r="20" spans="1:19">
-      <c r="A20" s="9"/>
+      <c r="A20" s="10"/>
       <c r="B20" s="2" t="s">
         <v>21</v>
       </c>
@@ -1746,16 +1760,15 @@
       <c r="O20" s="2">
         <v>0</v>
       </c>
-      <c r="P20" s="2">
-        <v>0</v>
+      <c r="P20" s="7" t="s">
+        <v>45</v>
       </c>
       <c r="S20">
-        <f>SUM(C20:P20)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:19">
-      <c r="A21" s="9"/>
+      <c r="A21" s="10"/>
       <c r="B21" s="2" t="s">
         <v>22</v>
       </c>
@@ -1790,23 +1803,23 @@
         <v>0</v>
       </c>
       <c r="M21" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N21" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O21" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P21" s="7" t="s">
         <v>44</v>
       </c>
       <c r="S21">
-        <v>5.5</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="22" spans="1:19">
-      <c r="A22" s="9"/>
+      <c r="A22" s="10"/>
       <c r="B22" s="7" t="s">
         <v>38</v>
       </c>
@@ -1843,10 +1856,10 @@
       <c r="M22" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="N22" s="7">
-        <v>0</v>
-      </c>
-      <c r="O22" s="7">
+      <c r="N22" s="2">
+        <v>0</v>
+      </c>
+      <c r="O22" s="2">
         <v>0</v>
       </c>
       <c r="P22" s="7" t="s">
@@ -1857,7 +1870,7 @@
       </c>
     </row>
     <row r="23" spans="1:19">
-      <c r="A23" s="9"/>
+      <c r="A23" s="10"/>
       <c r="B23" s="2" t="s">
         <v>24</v>
       </c>
@@ -1892,23 +1905,23 @@
         <v>0</v>
       </c>
       <c r="M23" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N23" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O23" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P23" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S23">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:19">
-      <c r="A24" s="9"/>
+      <c r="A24" s="10"/>
       <c r="B24" s="2" t="s">
         <v>25</v>
       </c>
@@ -1949,14 +1962,14 @@
         <v>0</v>
       </c>
       <c r="O24" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P24" s="2">
         <v>0</v>
       </c>
       <c r="S24">
         <f>SUM(C24:P24)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:19">
@@ -1995,18 +2008,18 @@
         <v>3</v>
       </c>
       <c r="M27" s="4">
-        <v>7</v>
+        <v>2.5</v>
       </c>
       <c r="N27" s="4">
-        <f t="shared" ref="C27:P27" si="2">SUM(N18:N24)</f>
-        <v>3</v>
+        <f t="shared" ref="N27:O27" si="2">SUM(N18:N24)</f>
+        <v>0</v>
       </c>
       <c r="O27" s="4">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="P27" s="4">
-        <v>7</v>
+        <v>7.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made Revised System Design, Updated Burndown Chart
Removed prototype, changed backlog numbers a little
</commit_message>
<xml_diff>
--- a/D3/Sprint #1 - Sprint Backlog.xlsx
+++ b/D3/Sprint #1 - Sprint Backlog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mitko\Documents\team14-course-project\D3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nanson\Desktop\Homework\University\CSCC01\team14-course-project\D3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -472,7 +472,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -607,10 +607,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1028,10 +1028,10 @@
   <dimension ref="A1:S27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S24" sqref="S24"/>
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.7109375" customWidth="1"/>
     <col min="2" max="2" width="44.28515625" customWidth="1"/>
@@ -1039,12 +1039,12 @@
     <col min="19" max="19" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="14.45" customHeight="1">
+    <row r="2" spans="1:19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1097,8 +1097,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1151,8 +1151,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="15" customHeight="1">
-      <c r="A4" s="9"/>
+    <row r="4" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
       <c r="B4" s="2" t="s">
         <v>20</v>
       </c>
@@ -1203,8 +1203,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
-      <c r="A5" s="9"/>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
       <c r="B5" s="2" t="s">
         <v>21</v>
       </c>
@@ -1255,8 +1255,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
-      <c r="A6" s="9"/>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="10"/>
       <c r="B6" s="2" t="s">
         <v>22</v>
       </c>
@@ -1307,8 +1307,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
-      <c r="A7" s="9"/>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="10"/>
       <c r="B7" s="2" t="s">
         <v>23</v>
       </c>
@@ -1359,8 +1359,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
-      <c r="A8" s="9"/>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="10"/>
       <c r="B8" s="2" t="s">
         <v>24</v>
       </c>
@@ -1411,8 +1411,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
-      <c r="A9" s="9"/>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="10"/>
       <c r="B9" s="2" t="s">
         <v>25</v>
       </c>
@@ -1463,7 +1463,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>26</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>27</v>
       </c>
@@ -1534,18 +1534,18 @@
         <v>97</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>28</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="H16" s="10" t="s">
+      <c r="H16" s="9" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:19">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>1</v>
       </c>
@@ -1598,8 +1598,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="15" customHeight="1">
-      <c r="A18" s="9" t="s">
+    <row r="18" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
         <v>18</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -1636,23 +1636,23 @@
         <v>34</v>
       </c>
       <c r="M18" s="2">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="N18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S18">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="15" customHeight="1">
-      <c r="A19" s="9"/>
+    <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="10"/>
       <c r="B19" s="2" t="s">
         <v>20</v>
       </c>
@@ -1687,7 +1687,7 @@
         <v>35</v>
       </c>
       <c r="M19" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N19" s="7">
         <v>0</v>
@@ -1702,8 +1702,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:19">
-      <c r="A20" s="9"/>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A20" s="10"/>
       <c r="B20" s="2" t="s">
         <v>21</v>
       </c>
@@ -1754,8 +1754,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:19">
-      <c r="A21" s="9"/>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A21" s="10"/>
       <c r="B21" s="2" t="s">
         <v>22</v>
       </c>
@@ -1790,13 +1790,13 @@
         <v>0</v>
       </c>
       <c r="M21" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N21" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O21" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P21" s="7" t="s">
         <v>44</v>
@@ -1805,8 +1805,8 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="22" spans="1:19">
-      <c r="A22" s="9"/>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A22" s="10"/>
       <c r="B22" s="7" t="s">
         <v>38</v>
       </c>
@@ -1856,8 +1856,8 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="23" spans="1:19">
-      <c r="A23" s="9"/>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A23" s="10"/>
       <c r="B23" s="2" t="s">
         <v>24</v>
       </c>
@@ -1892,23 +1892,23 @@
         <v>0</v>
       </c>
       <c r="M23" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N23" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O23" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P23" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S23">
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:19">
-      <c r="A24" s="9"/>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A24" s="10"/>
       <c r="B24" s="2" t="s">
         <v>25</v>
       </c>
@@ -1949,17 +1949,17 @@
         <v>0</v>
       </c>
       <c r="O24" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P24" s="2">
         <v>0</v>
       </c>
       <c r="S24">
         <f>SUM(C24:P24)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:19">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
@@ -1995,18 +1995,18 @@
         <v>3</v>
       </c>
       <c r="M27" s="4">
-        <v>7</v>
+        <v>2.5</v>
       </c>
       <c r="N27" s="4">
-        <f t="shared" ref="C27:P27" si="2">SUM(N18:N24)</f>
-        <v>3</v>
+        <f t="shared" ref="N27:O27" si="2">SUM(N18:N24)</f>
+        <v>0</v>
       </c>
       <c r="O27" s="4">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="P27" s="4">
-        <v>7</v>
+        <v>5.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Sprint Backlog, Burndown Chart, Documentation
</commit_message>
<xml_diff>
--- a/D3/Sprint #1 - Sprint Backlog.xlsx
+++ b/D3/Sprint #1 - Sprint Backlog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="46">
   <si>
     <t>Estimated</t>
   </si>
@@ -466,6 +466,21 @@
       </rPr>
       <t>2.5</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">N: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <phoneticPr fontId="6"/>
   </si>
 </sst>
 </file>
@@ -1027,8 +1042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="S27" sqref="S27"/>
+    <sheetView tabSelected="1" topLeftCell="B14" workbookViewId="0">
+      <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1951,12 +1966,11 @@
       <c r="O24" s="2">
         <v>0</v>
       </c>
-      <c r="P24" s="2">
-        <v>0</v>
+      <c r="P24" s="7" t="s">
+        <v>45</v>
       </c>
       <c r="S24">
-        <f>SUM(C24:P24)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
@@ -2006,7 +2020,7 @@
         <v>0</v>
       </c>
       <c r="P27" s="4">
-        <v>5.5</v>
+        <v>10.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Linux compatibility, separated Javascript from XUL, removed unnecessary code and renamed hello.js
</commit_message>
<xml_diff>
--- a/D3/Sprint #1 - Sprint Backlog.xlsx
+++ b/D3/Sprint #1 - Sprint Backlog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nanson\Desktop\Homework\University\CSCC01\team14-course-project\D3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows\Documents\GitHub\team14-course-project\D3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="50">
   <si>
     <t>Estimated</t>
   </si>
@@ -481,13 +481,58 @@
       <t>5</t>
     </r>
     <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>Task #6 Incorporation of javascript and gui</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">v: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>v:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>v:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -678,7 +723,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table5212" displayName="Table5212" ref="B17:P24" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table5212" displayName="Table5212" ref="B17:P25" headerRowCount="0">
   <tableColumns count="15">
     <tableColumn id="1" name="Column1"/>
     <tableColumn id="2" name="Column2"/>
@@ -1043,10 +1088,10 @@
   <dimension ref="A1:S27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B14" workbookViewId="0">
-      <selection activeCell="P28" sqref="P28"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.7109375" customWidth="1"/>
     <col min="2" max="2" width="44.28515625" customWidth="1"/>
@@ -1054,12 +1099,12 @@
     <col min="19" max="19" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="14.45" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1112,7 +1157,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" s="10" t="s">
         <v>18</v>
       </c>
@@ -1166,7 +1211,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="15" customHeight="1">
       <c r="A4" s="10"/>
       <c r="B4" s="2" t="s">
         <v>20</v>
@@ -1218,7 +1263,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19">
       <c r="A5" s="10"/>
       <c r="B5" s="2" t="s">
         <v>21</v>
@@ -1270,7 +1315,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19">
       <c r="A6" s="10"/>
       <c r="B6" s="2" t="s">
         <v>22</v>
@@ -1322,7 +1367,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19">
       <c r="A7" s="10"/>
       <c r="B7" s="2" t="s">
         <v>23</v>
@@ -1374,7 +1419,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19">
       <c r="A8" s="10"/>
       <c r="B8" s="2" t="s">
         <v>24</v>
@@ -1426,7 +1471,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19">
       <c r="A9" s="10"/>
       <c r="B9" s="2" t="s">
         <v>25</v>
@@ -1478,7 +1523,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19">
       <c r="A12" s="3" t="s">
         <v>26</v>
       </c>
@@ -1540,7 +1585,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19">
       <c r="A14" s="5" t="s">
         <v>27</v>
       </c>
@@ -1549,7 +1594,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -1560,7 +1605,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19">
       <c r="A17" s="1" t="s">
         <v>1</v>
       </c>
@@ -1613,7 +1658,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" ht="15" customHeight="1">
       <c r="A18" s="10" t="s">
         <v>18</v>
       </c>
@@ -1666,7 +1711,7 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" ht="15" customHeight="1">
       <c r="A19" s="10"/>
       <c r="B19" s="2" t="s">
         <v>20</v>
@@ -1717,7 +1762,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19">
       <c r="A20" s="10"/>
       <c r="B20" s="2" t="s">
         <v>21</v>
@@ -1769,7 +1814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19">
       <c r="A21" s="10"/>
       <c r="B21" s="2" t="s">
         <v>22</v>
@@ -1820,7 +1865,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19">
       <c r="A22" s="10"/>
       <c r="B22" s="7" t="s">
         <v>38</v>
@@ -1871,7 +1916,7 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19">
       <c r="A23" s="10"/>
       <c r="B23" s="2" t="s">
         <v>24</v>
@@ -1922,7 +1967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19">
       <c r="A24" s="10"/>
       <c r="B24" s="2" t="s">
         <v>25</v>
@@ -1973,7 +2018,24 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19">
+      <c r="B25" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19">
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>

</xml_diff>